<commit_message>
updated for manual false pos/false neg scoring with smaller set of uploaded data available
</commit_message>
<xml_diff>
--- a/2018-11-15 qbic test 2a.xlsx
+++ b/2018-11-15 qbic test 2a.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/theresa/Documents/home-github/cellprofiler/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C462F10C-1F18-F447-B13E-07775E4E84D8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04F9E262-7F6F-184B-867B-C5445202CD52}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2680" yWindow="6700" windowWidth="24780" windowHeight="10480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="820" yWindow="6700" windowWidth="24780" windowHeight="10480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2018-11-15 qbic test 2" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Image</t>
   </si>
@@ -37,10 +37,16 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>look to be actually 7 cells in the frame -- AP detected 2 false pos. too</t>
+    <t>CP count based on looking at obj image for this point and below</t>
   </si>
   <si>
-    <t>Analyze particles based on bad mask</t>
+    <t>1 possible false pos (out of focus) lower right</t>
+  </si>
+  <si>
+    <t>Edge objects inconsistent -- here a cell was detected that is at edge (partial nucleus) but in #43 a cell barely on edge was eliminated</t>
+  </si>
+  <si>
+    <t>false pos = elongated junk</t>
   </si>
 </sst>
 </file>
@@ -884,8 +890,8 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E1" sqref="E1:E1048576"/>
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -949,7 +955,7 @@
         <v>0</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -965,9 +971,6 @@
       <c r="D5">
         <v>0</v>
       </c>
-      <c r="E5" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
@@ -982,9 +985,6 @@
       <c r="D6">
         <v>0</v>
       </c>
-      <c r="E6" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
@@ -1004,50 +1004,152 @@
       <c r="A8">
         <v>2</v>
       </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>12</v>
       </c>
+      <c r="B9">
+        <v>9</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>7</v>
       </c>
+      <c r="B10">
+        <v>13</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>45</v>
       </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>43</v>
       </c>
+      <c r="B12">
+        <v>16</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>31</v>
       </c>
+      <c r="B13">
+        <v>12</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>32</v>
       </c>
+      <c r="B14">
+        <v>15</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>29</v>
       </c>
+      <c r="B15">
+        <v>10</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>30</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B16">
+        <v>14</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>39</v>
+      </c>
+      <c r="B17">
+        <v>9</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating most recent test data
</commit_message>
<xml_diff>
--- a/2018-11-15 qbic test 2a.xlsx
+++ b/2018-11-15 qbic test 2a.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/theresa/Documents/home-github/cellprofiler/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/confocal/github_theresaswayne/cellprofiler/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04F9E262-7F6F-184B-867B-C5445202CD52}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D11EDDBD-C26A-514A-9AD7-E8ABDAC672D9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="820" yWindow="6700" windowWidth="24780" windowHeight="10480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1360" yWindow="1840" windowWidth="24780" windowHeight="14600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2018-11-15 qbic test 2" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Image</t>
   </si>
@@ -47,6 +47,9 @@
   </si>
   <si>
     <t>false pos = elongated junk</t>
+  </si>
+  <si>
+    <t>one cell near top edge was segmented smaller than in reality</t>
   </si>
 </sst>
 </file>
@@ -887,11 +890,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1138,7 +1141,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>39</v>
       </c>
@@ -1150,6 +1153,65 @@
       </c>
       <c r="D17">
         <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>68</v>
+      </c>
+      <c r="B18">
+        <v>15</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>85</v>
+      </c>
+      <c r="B19">
+        <v>8</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>65</v>
+      </c>
+      <c r="B20">
+        <v>3</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>86</v>
+      </c>
+      <c r="B21">
+        <v>8</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>